<commit_message>
Updated to fix the disciplinary issue for edit the case status
</commit_message>
<xml_diff>
--- a/test-resources/HRM_TestData.xlsx
+++ b/test-resources/HRM_TestData.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\SeleniumLectures\SeleniumAutomation\test-resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C4506D-1025-41BC-BFEE-EDB8DDF365ED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B824136E-C171-4238-B3F6-EB34CD387E58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="19455" windowHeight="11820" tabRatio="773" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -23,7 +18,8 @@
     <sheet name="Add User Cases" sheetId="5" r:id="rId8"/>
     <sheet name="Travel_Request" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:I7"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="433">
   <si>
     <t>Seriel No</t>
   </si>
@@ -1190,9 +1186,6 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>Dashboard is not available, Test case is failed</t>
-  </si>
-  <si>
     <t>May/18/2020</t>
   </si>
   <si>
@@ -1314,6 +1307,30 @@
   </si>
   <si>
     <t>FionaxSRf</t>
+  </si>
+  <si>
+    <t>Amanda Cooper is not validated, Test case is failed</t>
+  </si>
+  <si>
+    <t>In Progress is not validated, Test case is failed</t>
+  </si>
+  <si>
+    <t>Fiona Grace</t>
+  </si>
+  <si>
+    <t>Jacqueline White</t>
+  </si>
+  <si>
+    <t>Mon, 27 Apr 2020</t>
+  </si>
+  <si>
+    <t>Khloe Jayden</t>
+  </si>
+  <si>
+    <t>Ehioze Ebo</t>
+  </si>
+  <si>
+    <t>Tue, 28 Apr 2020</t>
   </si>
 </sst>
 </file>
@@ -1518,10 +1535,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1749,18 +1766,18 @@
   </sheetPr>
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:B55"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.6328125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="50.08984375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="50.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1786,19 +1803,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1817,8 +1834,14 @@
       <c r="F3" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>368</v>
+      </c>
+      <c r="H3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1838,7 +1861,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1858,7 +1881,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1878,7 +1901,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1898,7 +1921,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1918,7 +1941,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1938,7 +1961,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1958,7 +1981,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1978,7 +2001,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1997,20 +2020,26 @@
       <c r="F12" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="G12" t="s">
+        <v>368</v>
+      </c>
+      <c r="H12" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -2036,7 +2065,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>2</v>
       </c>
@@ -2056,7 +2085,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -2076,7 +2105,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -2096,7 +2125,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -2116,7 +2145,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>6</v>
       </c>
@@ -2136,7 +2165,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>7</v>
       </c>
@@ -2156,7 +2185,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>8</v>
       </c>
@@ -2176,7 +2205,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>9</v>
       </c>
@@ -2196,7 +2225,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>10</v>
       </c>
@@ -2216,19 +2245,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+    <row r="24" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-    </row>
-    <row r="25" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+    </row>
+    <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>1</v>
       </c>
@@ -2248,7 +2277,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>2</v>
       </c>
@@ -2268,7 +2297,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>3</v>
       </c>
@@ -2288,7 +2317,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>4</v>
       </c>
@@ -2308,7 +2337,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>5</v>
       </c>
@@ -2328,7 +2357,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>6</v>
       </c>
@@ -2348,7 +2377,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>7</v>
       </c>
@@ -2368,7 +2397,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>8</v>
       </c>
@@ -2388,7 +2417,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>9</v>
       </c>
@@ -2408,7 +2437,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>10</v>
       </c>
@@ -2428,19 +2457,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
+    <row r="35" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-    </row>
-    <row r="36" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+    </row>
+    <row r="36" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>1</v>
       </c>
@@ -2466,7 +2495,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>2</v>
       </c>
@@ -2486,7 +2515,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>3</v>
       </c>
@@ -2506,7 +2535,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>4</v>
       </c>
@@ -2526,7 +2555,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>5</v>
       </c>
@@ -2546,7 +2575,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>6</v>
       </c>
@@ -2566,7 +2595,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>7</v>
       </c>
@@ -2586,7 +2615,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>8</v>
       </c>
@@ -2606,7 +2635,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>9</v>
       </c>
@@ -2626,7 +2655,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>10</v>
       </c>
@@ -2646,19 +2675,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="31" t="s">
+    <row r="46" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-    </row>
-    <row r="47" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+    </row>
+    <row r="47" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
         <v>1</v>
       </c>
@@ -2678,13 +2707,13 @@
         <v>30</v>
       </c>
       <c r="G47" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="H47" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8">
         <v>2</v>
       </c>
@@ -2704,7 +2733,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8">
         <v>3</v>
       </c>
@@ -2724,7 +2753,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <v>4</v>
       </c>
@@ -2744,7 +2773,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
         <v>5</v>
       </c>
@@ -2764,7 +2793,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
         <v>6</v>
       </c>
@@ -2784,7 +2813,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
         <v>7</v>
       </c>
@@ -2804,7 +2833,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
         <v>8</v>
       </c>
@@ -2824,7 +2853,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="8">
         <v>9</v>
       </c>
@@ -2844,7 +2873,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
         <v>10</v>
       </c>
@@ -2864,19 +2893,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="31" t="s">
+    <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="B57" s="31"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="31"/>
-      <c r="H57" s="31"/>
-    </row>
-    <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="32"/>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <v>1</v>
       </c>
@@ -2902,7 +2931,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <v>2</v>
       </c>
@@ -2922,7 +2951,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>3</v>
       </c>
@@ -2942,7 +2971,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="8">
         <v>4</v>
       </c>
@@ -2962,7 +2991,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="8">
         <v>5</v>
       </c>
@@ -2982,7 +3011,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <v>6</v>
       </c>
@@ -3002,7 +3031,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="8">
         <v>7</v>
       </c>
@@ -3022,7 +3051,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
         <v>8</v>
       </c>
@@ -3042,7 +3071,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="8">
         <v>9</v>
       </c>
@@ -3062,7 +3091,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="8">
         <v>10</v>
       </c>
@@ -3082,19 +3111,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="31" t="s">
+    <row r="68" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="32" t="s">
         <v>336</v>
       </c>
-      <c r="B68" s="31"/>
-      <c r="C68" s="31"/>
-      <c r="D68" s="31"/>
-      <c r="E68" s="31"/>
-      <c r="F68" s="31"/>
-      <c r="G68" s="31"/>
-      <c r="H68" s="31"/>
-    </row>
-    <row r="69" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="32"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="32"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="32"/>
+      <c r="G68" s="32"/>
+      <c r="H68" s="32"/>
+    </row>
+    <row r="69" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="8">
         <v>1</v>
       </c>
@@ -3120,7 +3149,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="8">
         <v>2</v>
       </c>
@@ -3146,7 +3175,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="8">
         <v>3</v>
       </c>
@@ -3166,7 +3195,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="8">
         <v>4</v>
       </c>
@@ -3186,7 +3215,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="8">
         <v>5</v>
       </c>
@@ -3206,7 +3235,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="8">
         <v>6</v>
       </c>
@@ -3307,16 +3336,16 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="31" t="s">
+      <c r="A79" s="32" t="s">
         <v>339</v>
       </c>
-      <c r="B79" s="31"/>
-      <c r="C79" s="31"/>
-      <c r="D79" s="31"/>
-      <c r="E79" s="31"/>
-      <c r="F79" s="31"/>
-      <c r="G79" s="31"/>
-      <c r="H79" s="31"/>
+      <c r="B79" s="32"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="32"/>
+      <c r="E79" s="32"/>
+      <c r="F79" s="32"/>
+      <c r="G79" s="32"/>
+      <c r="H79" s="32"/>
     </row>
     <row r="80" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
@@ -3542,22 +3571,22 @@
       <selection activeCell="I2" sqref="I2:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.6328125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="10.90625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.26953125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="28.6328125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="27.453125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.453125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="19.6328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>203</v>
       </c>
@@ -3604,7 +3633,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -3651,7 +3680,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>59</v>
       </c>
@@ -3698,7 +3727,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>72</v>
       </c>
@@ -3745,7 +3774,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>80</v>
       </c>
@@ -3792,7 +3821,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>91</v>
       </c>
@@ -3839,7 +3868,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>97</v>
       </c>
@@ -3886,7 +3915,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>103</v>
       </c>
@@ -3933,7 +3962,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>109</v>
       </c>
@@ -3980,7 +4009,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>115</v>
       </c>
@@ -4027,7 +4056,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>122</v>
       </c>
@@ -4092,18 +4121,18 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.26953125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="19.36328125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.08984375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>203</v>
       </c>
@@ -4129,7 +4158,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -4146,13 +4175,13 @@
         <v>43</v>
       </c>
       <c r="F2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L2" t="s">
         <v>389</v>
       </c>
-      <c r="L2" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>59</v>
       </c>
@@ -4169,7 +4198,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>72</v>
       </c>
@@ -4186,7 +4215,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>80</v>
       </c>
@@ -4203,7 +4232,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>91</v>
       </c>
@@ -4220,7 +4249,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>97</v>
       </c>
@@ -4237,7 +4266,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>103</v>
       </c>
@@ -4254,7 +4283,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>109</v>
       </c>
@@ -4271,7 +4300,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>115</v>
       </c>
@@ -4288,7 +4317,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>122</v>
       </c>
@@ -4323,21 +4352,21 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.54296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.1796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="21.26953125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="25.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="21.36328125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>203</v>
       </c>
@@ -4372,7 +4401,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -4389,7 +4418,7 @@
         <v>43</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>282</v>
@@ -4407,7 +4436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>59</v>
       </c>
@@ -4442,7 +4471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>72</v>
       </c>
@@ -4477,7 +4506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>80</v>
       </c>
@@ -4512,7 +4541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>91</v>
       </c>
@@ -4547,7 +4576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>97</v>
       </c>
@@ -4582,7 +4611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>103</v>
       </c>
@@ -4617,7 +4646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>109</v>
       </c>
@@ -4652,7 +4681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>115</v>
       </c>
@@ -4687,7 +4716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>122</v>
       </c>
@@ -4741,18 +4770,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="24.26953125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.28515625" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.81640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="19.54296875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="20.7265625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.453125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="14.08984375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -4787,7 +4816,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>18</v>
       </c>
@@ -4822,7 +4851,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>59</v>
       </c>
@@ -4857,7 +4886,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>72</v>
       </c>
@@ -4892,7 +4921,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>80</v>
       </c>
@@ -4927,7 +4956,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>91</v>
       </c>
@@ -4962,7 +4991,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>97</v>
       </c>
@@ -4997,7 +5026,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>103</v>
       </c>
@@ -5032,7 +5061,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>109</v>
       </c>
@@ -5067,7 +5096,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>115</v>
       </c>
@@ -5102,7 +5131,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>122</v>
       </c>
@@ -5137,7 +5166,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23"/>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -5152,7 +5181,7 @@
       <c r="J12" s="23"/>
       <c r="K12" s="23"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="23"/>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -5183,14 +5212,14 @@
       <selection sqref="A1:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="24.26953125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.81640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -5219,7 +5248,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>18</v>
       </c>
@@ -5238,17 +5267,17 @@
       <c r="F2" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="31" t="s">
+        <v>391</v>
+      </c>
+      <c r="H2" s="31" t="s">
         <v>392</v>
-      </c>
-      <c r="H2" s="34" t="s">
-        <v>393</v>
       </c>
       <c r="I2" s="27" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>59</v>
       </c>
@@ -5267,17 +5296,17 @@
       <c r="F3" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="31" t="s">
+        <v>391</v>
+      </c>
+      <c r="H3" s="31" t="s">
         <v>392</v>
-      </c>
-      <c r="H3" s="34" t="s">
-        <v>393</v>
       </c>
       <c r="I3" s="27" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>72</v>
       </c>
@@ -5296,17 +5325,17 @@
       <c r="F4" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="31" t="s">
+        <v>393</v>
+      </c>
+      <c r="H4" s="31" t="s">
         <v>394</v>
-      </c>
-      <c r="H4" s="34" t="s">
-        <v>395</v>
       </c>
       <c r="I4" s="27" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>80</v>
       </c>
@@ -5325,17 +5354,17 @@
       <c r="F5" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="31" t="s">
+        <v>395</v>
+      </c>
+      <c r="H5" s="31" t="s">
         <v>396</v>
-      </c>
-      <c r="H5" s="34" t="s">
-        <v>397</v>
       </c>
       <c r="I5" s="27" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>91</v>
       </c>
@@ -5354,17 +5383,17 @@
       <c r="F6" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="G6" s="34" t="s">
+      <c r="G6" s="31" t="s">
+        <v>397</v>
+      </c>
+      <c r="H6" s="31" t="s">
         <v>398</v>
-      </c>
-      <c r="H6" s="34" t="s">
-        <v>399</v>
       </c>
       <c r="I6" s="27" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>97</v>
       </c>
@@ -5383,17 +5412,17 @@
       <c r="F7" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="G7" s="34" t="s">
-        <v>400</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>396</v>
+      <c r="G7" s="31" t="s">
+        <v>399</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>395</v>
       </c>
       <c r="I7" s="27" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>103</v>
       </c>
@@ -5412,17 +5441,17 @@
       <c r="F8" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="G8" s="34" t="s">
-        <v>401</v>
-      </c>
-      <c r="H8" s="34" t="s">
-        <v>396</v>
+      <c r="G8" s="31" t="s">
+        <v>400</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>395</v>
       </c>
       <c r="I8" s="27" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>109</v>
       </c>
@@ -5441,17 +5470,17 @@
       <c r="F9" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="G9" s="34" t="s">
+      <c r="G9" s="31" t="s">
+        <v>401</v>
+      </c>
+      <c r="H9" s="31" t="s">
         <v>402</v>
-      </c>
-      <c r="H9" s="34" t="s">
-        <v>403</v>
       </c>
       <c r="I9" s="27" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>115</v>
       </c>
@@ -5470,17 +5499,17 @@
       <c r="F10" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="G10" s="34" t="s">
-        <v>401</v>
-      </c>
-      <c r="H10" s="34" t="s">
-        <v>396</v>
+      <c r="G10" s="31" t="s">
+        <v>400</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>395</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>122</v>
       </c>
@@ -5499,11 +5528,11 @@
       <c r="F11" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="31" t="s">
+        <v>403</v>
+      </c>
+      <c r="H11" s="31" t="s">
         <v>404</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>405</v>
       </c>
       <c r="I11" s="27" t="s">
         <v>168</v>
@@ -5521,24 +5550,24 @@
   </sheetPr>
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="30" width="14.453125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="30" width="22.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="30" width="11.26953125" collapsed="true"/>
-    <col min="4" max="6" style="30" width="14.453125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="30" width="23.08984375" collapsed="true"/>
-    <col min="8" max="9" style="30" width="14.453125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="30" width="29.7265625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="30" width="17.7265625" collapsed="true"/>
-    <col min="12" max="16384" style="30" width="14.453125" collapsed="true"/>
+    <col min="1" max="1" style="30" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="30" width="22.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="30" width="11.28515625" collapsed="true"/>
+    <col min="4" max="6" style="30" width="14.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="30" width="23.140625" collapsed="true"/>
+    <col min="8" max="9" style="30" width="14.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="30" width="29.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="30" width="17.7109375" collapsed="true"/>
+    <col min="12" max="16384" style="30" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -5582,7 +5611,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>18</v>
       </c>
@@ -5602,7 +5631,7 @@
         <v>44</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H2" s="25" t="s">
         <v>47</v>
@@ -5614,13 +5643,19 @@
         <v>50</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>57</v>
+        <v>292</v>
       </c>
       <c r="L2" s="27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+      <c r="M2" t="s">
+        <v>428</v>
+      </c>
+      <c r="N2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>59</v>
       </c>
@@ -5640,10 +5675,10 @@
         <v>65</v>
       </c>
       <c r="G3" s="28" t="s">
+        <v>406</v>
+      </c>
+      <c r="H3" s="31" t="s">
         <v>407</v>
-      </c>
-      <c r="H3" s="34" t="s">
-        <v>408</v>
       </c>
       <c r="I3" s="27" t="s">
         <v>66</v>
@@ -5655,7 +5690,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>72</v>
       </c>
@@ -5675,10 +5710,10 @@
         <v>73</v>
       </c>
       <c r="G4" s="28" t="s">
+        <v>408</v>
+      </c>
+      <c r="H4" s="31" t="s">
         <v>409</v>
-      </c>
-      <c r="H4" s="34" t="s">
-        <v>410</v>
       </c>
       <c r="I4" s="27" t="s">
         <v>77</v>
@@ -5687,7 +5722,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>80</v>
       </c>
@@ -5707,10 +5742,10 @@
         <v>87</v>
       </c>
       <c r="G5" s="28" t="s">
+        <v>410</v>
+      </c>
+      <c r="H5" s="31" t="s">
         <v>411</v>
-      </c>
-      <c r="H5" s="34" t="s">
-        <v>412</v>
       </c>
       <c r="I5" s="27" t="s">
         <v>48</v>
@@ -5719,7 +5754,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>91</v>
       </c>
@@ -5739,10 +5774,10 @@
         <v>93</v>
       </c>
       <c r="G6" s="28" t="s">
+        <v>412</v>
+      </c>
+      <c r="H6" s="31" t="s">
         <v>413</v>
-      </c>
-      <c r="H6" s="34" t="s">
-        <v>414</v>
       </c>
       <c r="I6" s="27" t="s">
         <v>66</v>
@@ -5751,7 +5786,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>97</v>
       </c>
@@ -5771,10 +5806,10 @@
         <v>100</v>
       </c>
       <c r="G7" s="28" t="s">
+        <v>414</v>
+      </c>
+      <c r="H7" s="31" t="s">
         <v>415</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>416</v>
       </c>
       <c r="I7" s="27" t="s">
         <v>77</v>
@@ -5783,7 +5818,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>103</v>
       </c>
@@ -5803,10 +5838,10 @@
         <v>106</v>
       </c>
       <c r="G8" s="28" t="s">
+        <v>416</v>
+      </c>
+      <c r="H8" s="31" t="s">
         <v>417</v>
-      </c>
-      <c r="H8" s="34" t="s">
-        <v>418</v>
       </c>
       <c r="I8" s="27" t="s">
         <v>48</v>
@@ -5815,7 +5850,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>109</v>
       </c>
@@ -5835,10 +5870,10 @@
         <v>110</v>
       </c>
       <c r="G9" s="28" t="s">
+        <v>418</v>
+      </c>
+      <c r="H9" s="31" t="s">
         <v>419</v>
-      </c>
-      <c r="H9" s="34" t="s">
-        <v>420</v>
       </c>
       <c r="I9" s="27" t="s">
         <v>66</v>
@@ -5847,7 +5882,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>115</v>
       </c>
@@ -5867,10 +5902,10 @@
         <v>117</v>
       </c>
       <c r="G10" s="28" t="s">
+        <v>420</v>
+      </c>
+      <c r="H10" s="31" t="s">
         <v>421</v>
-      </c>
-      <c r="H10" s="34" t="s">
-        <v>422</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>77</v>
@@ -5879,7 +5914,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>122</v>
       </c>
@@ -5899,10 +5934,10 @@
         <v>124</v>
       </c>
       <c r="G11" s="28" t="s">
+        <v>422</v>
+      </c>
+      <c r="H11" s="31" t="s">
         <v>423</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>424</v>
       </c>
       <c r="I11" s="27" t="s">
         <v>48</v>
@@ -5910,8 +5945,20 @@
       <c r="J11" s="27" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>430</v>
+      </c>
+      <c r="L11" t="s">
+        <v>431</v>
+      </c>
+      <c r="M11" t="s">
+        <v>428</v>
+      </c>
+      <c r="N11" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
         <v>57</v>
       </c>
@@ -5939,7 +5986,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I13" s="27" t="s">
         <v>57</v>
       </c>
@@ -5960,14 +6007,14 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" style="30" width="14.453125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="30" width="17.453125" collapsed="true"/>
-    <col min="7" max="16384" style="30" width="14.453125" collapsed="true"/>
+    <col min="1" max="5" style="30" width="14.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="30" width="17.42578125" collapsed="true"/>
+    <col min="7" max="16384" style="30" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -5993,7 +6040,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>18</v>
       </c>
@@ -6016,10 +6063,10 @@
         <v>172</v>
       </c>
       <c r="H2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>59</v>
       </c>
@@ -6042,7 +6089,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>72</v>
       </c>
@@ -6065,7 +6112,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>80</v>
       </c>
@@ -6088,7 +6135,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>91</v>
       </c>
@@ -6111,7 +6158,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>97</v>
       </c>
@@ -6134,7 +6181,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>103</v>
       </c>
@@ -6157,7 +6204,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>109</v>
       </c>
@@ -6180,7 +6227,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>115</v>
       </c>
@@ -6203,7 +6250,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>122</v>
       </c>
@@ -6239,25 +6286,25 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.1796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.08984375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="27.54296875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="8.36328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>203</v>
       </c>
@@ -6304,7 +6351,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -6324,10 +6371,10 @@
         <v>311</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>325</v>
@@ -6336,7 +6383,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>59</v>
       </c>
@@ -6356,10 +6403,10 @@
         <v>312</v>
       </c>
       <c r="G3" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="H3" s="22" t="s">
         <v>387</v>
-      </c>
-      <c r="H3" s="22" t="s">
-        <v>388</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>326</v>
@@ -6368,7 +6415,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>72</v>
       </c>
@@ -6400,7 +6447,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>80</v>
       </c>
@@ -6432,7 +6479,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>91</v>
       </c>
@@ -6464,7 +6511,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>97</v>
       </c>
@@ -6496,7 +6543,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>103</v>
       </c>
@@ -6528,7 +6575,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>109</v>
       </c>
@@ -6560,7 +6607,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>115</v>
       </c>
@@ -6592,7 +6639,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>122</v>
       </c>

</xml_diff>

<commit_message>
Added few changes in the Travel Request and Add Vacancy test cases.
</commit_message>
<xml_diff>
--- a/test-resources/HRM_TestData.xlsx
+++ b/test-resources/HRM_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\SeleniumLectures\SeleniumAutomation\test-resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aneesh\git\OrangeHRMAutomation\test-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C4506D-1025-41BC-BFEE-EDB8DDF365ED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7A832B-4B1C-491E-8267-C05EC3B3308A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="773" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="424">
   <si>
     <t>Seriel No</t>
   </si>
@@ -956,15 +956,6 @@
     <t>IT</t>
   </si>
   <si>
-    <t>Director</t>
-  </si>
-  <si>
-    <t>Manager</t>
-  </si>
-  <si>
-    <t>Executive</t>
-  </si>
-  <si>
     <t>Currency Name</t>
   </si>
   <si>
@@ -1193,27 +1184,12 @@
     <t>Dashboard is not available, Test case is failed</t>
   </si>
   <si>
-    <t>May/18/2020</t>
-  </si>
-  <si>
-    <t>May/15/2020</t>
-  </si>
-  <si>
-    <t>August/20/2020</t>
-  </si>
-  <si>
-    <t>August/25/2020</t>
-  </si>
-  <si>
     <t>United KingdomxvAguU</t>
   </si>
   <si>
     <t>+91 5</t>
   </si>
   <si>
-    <t>Clerk9963</t>
-  </si>
-  <si>
     <t>May/20/2020</t>
   </si>
   <si>
@@ -1314,6 +1290,24 @@
   </si>
   <si>
     <t>FionaxSRf</t>
+  </si>
+  <si>
+    <t>Existing Location Name</t>
+  </si>
+  <si>
+    <t>London Office</t>
+  </si>
+  <si>
+    <t>New York Sales Office</t>
+  </si>
+  <si>
+    <t>Texas R&amp;D</t>
+  </si>
+  <si>
+    <t>Sample Location</t>
+  </si>
+  <si>
+    <t>seleniumprep-trials65101.orangehrmlive.com is not validated, Test case is failed</t>
   </si>
 </sst>
 </file>
@@ -1505,9 +1499,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
@@ -1518,10 +1509,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1749,8 +1741,8 @@
   </sheetPr>
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:B55"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1787,16 +1779,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -1999,16 +1991,16 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -2030,10 +2022,10 @@
         <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="H14" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2217,16 +2209,16 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
     </row>
     <row r="25" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -2247,6 +2239,12 @@
       <c r="F25" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="G25" t="s">
+        <v>380</v>
+      </c>
+      <c r="H25" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="26" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -2429,16 +2427,16 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
     </row>
     <row r="36" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
@@ -2460,10 +2458,10 @@
         <v>30</v>
       </c>
       <c r="G36" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="H36" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -2647,16 +2645,16 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
     </row>
     <row r="47" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
@@ -2678,10 +2676,10 @@
         <v>30</v>
       </c>
       <c r="G47" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H47" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2865,16 +2863,16 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="31" t="s">
+      <c r="A57" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="B57" s="31"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="31"/>
-      <c r="H57" s="31"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="32"/>
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
@@ -2887,7 +2885,7 @@
         <v>264</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E58" s="9" t="s">
         <v>27</v>
@@ -2896,10 +2894,10 @@
         <v>30</v>
       </c>
       <c r="G58" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="H58" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2913,7 +2911,7 @@
         <v>262</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>202</v>
@@ -2933,7 +2931,7 @@
         <v>265</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E60" s="9" t="s">
         <v>34</v>
@@ -2953,7 +2951,7 @@
         <v>266</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E61" s="9" t="s">
         <v>40</v>
@@ -2973,7 +2971,7 @@
         <v>267</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>27</v>
@@ -2993,7 +2991,7 @@
         <v>268</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E63" s="9" t="s">
         <v>40</v>
@@ -3013,7 +3011,7 @@
         <v>269</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>64</v>
@@ -3033,7 +3031,7 @@
         <v>270</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E65" s="9" t="s">
         <v>27</v>
@@ -3053,7 +3051,7 @@
         <v>271</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E66" s="9" t="s">
         <v>27</v>
@@ -3073,7 +3071,7 @@
         <v>272</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>27</v>
@@ -3083,16 +3081,16 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="31" t="s">
-        <v>336</v>
-      </c>
-      <c r="B68" s="31"/>
-      <c r="C68" s="31"/>
-      <c r="D68" s="31"/>
-      <c r="E68" s="31"/>
-      <c r="F68" s="31"/>
-      <c r="G68" s="31"/>
-      <c r="H68" s="31"/>
+      <c r="A68" s="32" t="s">
+        <v>333</v>
+      </c>
+      <c r="B68" s="32"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="32"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="32"/>
+      <c r="G68" s="32"/>
+      <c r="H68" s="32"/>
     </row>
     <row r="69" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
@@ -3102,10 +3100,10 @@
         <v>260</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E69" t="s">
         <v>27</v>
@@ -3114,10 +3112,10 @@
         <v>30</v>
       </c>
       <c r="G69" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="H69" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3128,10 +3126,10 @@
         <v>260</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E70" t="s">
         <v>34</v>
@@ -3140,10 +3138,10 @@
         <v>30</v>
       </c>
       <c r="G70" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="H70" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3154,10 +3152,10 @@
         <v>260</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E71" t="s">
         <v>40</v>
@@ -3174,10 +3172,10 @@
         <v>260</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E72" t="s">
         <v>64</v>
@@ -3194,10 +3192,10 @@
         <v>260</v>
       </c>
       <c r="C73" s="20" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E73" t="s">
         <v>202</v>
@@ -3214,10 +3212,10 @@
         <v>260</v>
       </c>
       <c r="C74" s="20" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E74" t="s">
         <v>27</v>
@@ -3234,10 +3232,10 @@
         <v>260</v>
       </c>
       <c r="C75" s="20" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E75" t="s">
         <v>40</v>
@@ -3254,10 +3252,10 @@
         <v>260</v>
       </c>
       <c r="C76" s="20" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E76" t="s">
         <v>34</v>
@@ -3274,10 +3272,10 @@
         <v>260</v>
       </c>
       <c r="C77" s="20" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E77" t="s">
         <v>27</v>
@@ -3294,10 +3292,10 @@
         <v>260</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E78" t="s">
         <v>27</v>
@@ -3307,16 +3305,16 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="31" t="s">
-        <v>339</v>
-      </c>
-      <c r="B79" s="31"/>
-      <c r="C79" s="31"/>
-      <c r="D79" s="31"/>
-      <c r="E79" s="31"/>
-      <c r="F79" s="31"/>
-      <c r="G79" s="31"/>
-      <c r="H79" s="31"/>
+      <c r="A79" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="B79" s="32"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="32"/>
+      <c r="E79" s="32"/>
+      <c r="F79" s="32"/>
+      <c r="G79" s="32"/>
+      <c r="H79" s="32"/>
     </row>
     <row r="80" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
@@ -3326,10 +3324,10 @@
         <v>261</v>
       </c>
       <c r="C80" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E80" t="s">
         <v>27</v>
@@ -3346,10 +3344,10 @@
         <v>261</v>
       </c>
       <c r="C81" s="19" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E81" t="s">
         <v>34</v>
@@ -3366,10 +3364,10 @@
         <v>261</v>
       </c>
       <c r="C82" s="19" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E82" t="s">
         <v>27</v>
@@ -3386,10 +3384,10 @@
         <v>261</v>
       </c>
       <c r="C83" s="19" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E83" t="s">
         <v>64</v>
@@ -3406,10 +3404,10 @@
         <v>261</v>
       </c>
       <c r="C84" s="19" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E84" t="s">
         <v>202</v>
@@ -3426,10 +3424,10 @@
         <v>261</v>
       </c>
       <c r="C85" s="19" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E85" t="s">
         <v>40</v>
@@ -3446,10 +3444,10 @@
         <v>261</v>
       </c>
       <c r="C86" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="D86" s="8" t="s">
         <v>346</v>
-      </c>
-      <c r="D86" s="8" t="s">
-        <v>349</v>
       </c>
       <c r="E86" t="s">
         <v>27</v>
@@ -3466,10 +3464,10 @@
         <v>261</v>
       </c>
       <c r="C87" s="19" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E87" t="s">
         <v>27</v>
@@ -3486,10 +3484,10 @@
         <v>261</v>
       </c>
       <c r="C88" s="19" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E88" t="s">
         <v>34</v>
@@ -3506,10 +3504,10 @@
         <v>261</v>
       </c>
       <c r="C89" s="19" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E89" t="s">
         <v>27</v>
@@ -3539,7 +3537,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I11"/>
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3630,7 +3628,7 @@
         <v>225</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>242</v>
@@ -3642,13 +3640,13 @@
         <v>250</v>
       </c>
       <c r="M2" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="N2" s="21" t="s">
         <v>359</v>
       </c>
-      <c r="N2" s="21" t="s">
-        <v>362</v>
-      </c>
       <c r="O2" s="20" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -3677,7 +3675,7 @@
         <v>236</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>243</v>
@@ -3689,13 +3687,13 @@
         <v>251</v>
       </c>
       <c r="M3" s="20" t="s">
+        <v>357</v>
+      </c>
+      <c r="N3" s="21" t="s">
         <v>360</v>
       </c>
-      <c r="N3" s="21" t="s">
-        <v>363</v>
-      </c>
       <c r="O3" s="20" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -3724,7 +3722,7 @@
         <v>226</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>244</v>
@@ -3736,13 +3734,13 @@
         <v>252</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="N4" s="21" t="s">
         <v>18</v>
       </c>
       <c r="O4" s="20" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -3771,7 +3769,7 @@
         <v>235</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>245</v>
@@ -3783,13 +3781,13 @@
         <v>253</v>
       </c>
       <c r="M5" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="N5" s="21" t="s">
         <v>359</v>
       </c>
-      <c r="N5" s="21" t="s">
-        <v>362</v>
-      </c>
       <c r="O5" s="20" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -3818,7 +3816,7 @@
         <v>234</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>246</v>
@@ -3830,13 +3828,13 @@
         <v>254</v>
       </c>
       <c r="M6" s="20" t="s">
+        <v>357</v>
+      </c>
+      <c r="N6" s="21" t="s">
         <v>360</v>
       </c>
-      <c r="N6" s="21" t="s">
-        <v>363</v>
-      </c>
       <c r="O6" s="20" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -3865,7 +3863,7 @@
         <v>233</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>247</v>
@@ -3877,13 +3875,13 @@
         <v>255</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="N7" s="21" t="s">
         <v>18</v>
       </c>
       <c r="O7" s="20" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -3912,7 +3910,7 @@
         <v>232</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>248</v>
@@ -3924,13 +3922,13 @@
         <v>256</v>
       </c>
       <c r="M8" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="N8" s="21" t="s">
         <v>359</v>
       </c>
-      <c r="N8" s="21" t="s">
-        <v>362</v>
-      </c>
       <c r="O8" s="20" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -3959,7 +3957,7 @@
         <v>230</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>249</v>
@@ -3971,13 +3969,13 @@
         <v>257</v>
       </c>
       <c r="M9" s="20" t="s">
+        <v>357</v>
+      </c>
+      <c r="N9" s="21" t="s">
         <v>360</v>
       </c>
-      <c r="N9" s="21" t="s">
-        <v>363</v>
-      </c>
       <c r="O9" s="20" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -4006,7 +4004,7 @@
         <v>229</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>248</v>
@@ -4018,13 +4016,13 @@
         <v>258</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="N10" s="21" t="s">
         <v>18</v>
       </c>
       <c r="O10" s="20" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -4053,7 +4051,7 @@
         <v>228</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>243</v>
@@ -4065,13 +4063,13 @@
         <v>250</v>
       </c>
       <c r="M11" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="N11" s="21" t="s">
         <v>359</v>
       </c>
-      <c r="N11" s="21" t="s">
+      <c r="O11" s="20" t="s">
         <v>362</v>
-      </c>
-      <c r="O11" s="20" t="s">
-        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -4086,10 +4084,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A07C2E7-1AF9-4E6C-8A44-C55DF7F49724}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4098,12 +4096,13 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="19.36328125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.08984375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="30" width="25.453125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.36328125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.08984375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>203</v>
       </c>
@@ -4119,17 +4118,20 @@
       <c r="E1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -4145,14 +4147,17 @@
       <c r="E2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F2" t="s">
-        <v>389</v>
-      </c>
-      <c r="L2" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F2" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="G2" t="s">
+        <v>382</v>
+      </c>
+      <c r="M2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>59</v>
       </c>
@@ -4168,8 +4173,11 @@
       <c r="E3" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F3" s="10" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>72</v>
       </c>
@@ -4185,8 +4193,11 @@
       <c r="E4" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F4" s="10" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>80</v>
       </c>
@@ -4202,8 +4213,11 @@
       <c r="E5" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F5" s="10" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>91</v>
       </c>
@@ -4219,8 +4233,11 @@
       <c r="E6" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F6" s="10" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>97</v>
       </c>
@@ -4236,8 +4253,11 @@
       <c r="E7" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F7" s="10" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>103</v>
       </c>
@@ -4253,8 +4273,11 @@
       <c r="E8" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F8" s="10" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>109</v>
       </c>
@@ -4270,8 +4293,11 @@
       <c r="E9" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F9" s="10" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>115</v>
       </c>
@@ -4287,8 +4313,11 @@
       <c r="E10" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F10" s="10" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>122</v>
       </c>
@@ -4304,6 +4333,7 @@
       <c r="E11" s="10" t="s">
         <v>43</v>
       </c>
+      <c r="F11" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -4320,7 +4350,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F11" sqref="F2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4380,7 +4410,7 @@
         <v>260</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>41</v>
@@ -4388,14 +4418,12 @@
       <c r="E2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>391</v>
-      </c>
+      <c r="F2" s="15"/>
       <c r="G2" s="7" t="s">
         <v>282</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>299</v>
@@ -4415,7 +4443,7 @@
         <v>260</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>41</v>
@@ -4423,14 +4451,12 @@
       <c r="E3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>306</v>
-      </c>
+      <c r="F3" s="15"/>
       <c r="G3" s="7" t="s">
         <v>283</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>299</v>
@@ -4450,7 +4476,7 @@
         <v>260</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>41</v>
@@ -4458,14 +4484,12 @@
       <c r="E4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>307</v>
-      </c>
+      <c r="F4" s="15"/>
       <c r="G4" s="7" t="s">
         <v>284</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>300</v>
@@ -4485,7 +4509,7 @@
         <v>260</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>41</v>
@@ -4493,14 +4517,12 @@
       <c r="E5" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>307</v>
-      </c>
+      <c r="F5" s="15"/>
       <c r="G5" s="15" t="s">
         <v>285</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>305</v>
@@ -4520,7 +4542,7 @@
         <v>260</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>41</v>
@@ -4528,14 +4550,12 @@
       <c r="E6" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>286</v>
-      </c>
+      <c r="F6" s="15"/>
       <c r="G6" s="15" t="s">
         <v>286</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>300</v>
@@ -4555,7 +4575,7 @@
         <v>260</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>41</v>
@@ -4563,14 +4583,12 @@
       <c r="E7" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>307</v>
-      </c>
+      <c r="F7" s="15"/>
       <c r="G7" s="15" t="s">
         <v>287</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>297</v>
@@ -4590,7 +4608,7 @@
         <v>260</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>41</v>
@@ -4598,9 +4616,7 @@
       <c r="E8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>307</v>
-      </c>
+      <c r="F8" s="15"/>
       <c r="G8" s="15" t="s">
         <v>288</v>
       </c>
@@ -4625,7 +4641,7 @@
         <v>260</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>41</v>
@@ -4633,9 +4649,7 @@
       <c r="E9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>308</v>
-      </c>
+      <c r="F9" s="15"/>
       <c r="G9" s="15" t="s">
         <v>289</v>
       </c>
@@ -4660,7 +4674,7 @@
         <v>260</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>41</v>
@@ -4668,9 +4682,7 @@
       <c r="E10" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>307</v>
-      </c>
+      <c r="F10" s="15"/>
       <c r="G10" s="15" t="s">
         <v>290</v>
       </c>
@@ -4695,7 +4707,7 @@
         <v>260</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>41</v>
@@ -4703,9 +4715,7 @@
       <c r="E11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>308</v>
-      </c>
+      <c r="F11" s="15"/>
       <c r="G11" s="15" t="s">
         <v>291</v>
       </c>
@@ -4753,419 +4763,419 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="28" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="27" t="s">
+      <c r="D3" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="26" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="27" t="s">
+      <c r="D4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="26" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="27" t="s">
+      <c r="D5" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="K5" s="27" t="s">
+      <c r="K5" s="26" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="27" t="s">
+      <c r="D6" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="K6" s="29" t="s">
+      <c r="K6" s="28" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="27" t="s">
+      <c r="D7" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K7" s="27" t="s">
+      <c r="K7" s="26" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="D8" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="27" t="s">
+      <c r="D8" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="K8" s="26" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="27" t="s">
+      <c r="D9" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="K9" s="27" t="s">
+      <c r="K9" s="26" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="27" t="s">
+      <c r="D10" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="27" t="s">
+      <c r="I10" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="29" t="s">
+      <c r="K10" s="28" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="27" t="s">
+      <c r="D11" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I11" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K11" s="27" t="s">
+      <c r="K11" s="26" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="27" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="27" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5180,7 +5190,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I11"/>
+      <selection activeCell="G2" sqref="G2:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5191,321 +5201,321 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="23" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="29" t="s">
+      <c r="D2" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="31" t="s">
+        <v>384</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>385</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>384</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>385</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>386</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>387</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>388</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>389</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>390</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>391</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="G7" s="31" t="s">
         <v>392</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H7" s="31" t="s">
+        <v>388</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="G8" s="31" t="s">
         <v>393</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="H8" s="31" t="s">
+        <v>388</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>394</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>395</v>
+      </c>
+      <c r="I9" s="26" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="26" t="s">
+    <row r="10" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="G3" s="34" t="s">
-        <v>392</v>
-      </c>
-      <c r="H3" s="34" t="s">
+      <c r="C10" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="G10" s="31" t="s">
         <v>393</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="H10" s="31" t="s">
+        <v>388</v>
+      </c>
+      <c r="I10" s="26" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="26" t="s">
+    <row r="11" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>394</v>
-      </c>
-      <c r="H4" s="34" t="s">
-        <v>395</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>176</v>
-      </c>
-      <c r="G5" s="34" t="s">
+      <c r="C11" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="G11" s="31" t="s">
         <v>396</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H11" s="31" t="s">
         <v>397</v>
       </c>
-      <c r="I5" s="27" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>181</v>
-      </c>
-      <c r="G6" s="34" t="s">
-        <v>398</v>
-      </c>
-      <c r="H6" s="34" t="s">
-        <v>399</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="G7" s="34" t="s">
-        <v>400</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>396</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="G8" s="34" t="s">
-        <v>401</v>
-      </c>
-      <c r="H8" s="34" t="s">
-        <v>396</v>
-      </c>
-      <c r="I8" s="27" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="G9" s="34" t="s">
-        <v>402</v>
-      </c>
-      <c r="H9" s="34" t="s">
-        <v>403</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="G10" s="34" t="s">
-        <v>401</v>
-      </c>
-      <c r="H10" s="34" t="s">
-        <v>396</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="G11" s="34" t="s">
-        <v>404</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>405</v>
-      </c>
-      <c r="I11" s="27" t="s">
+      <c r="I11" s="26" t="s">
         <v>168</v>
       </c>
     </row>
@@ -5527,46 +5537,46 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="30" width="14.453125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="30" width="22.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="30" width="11.26953125" collapsed="true"/>
-    <col min="4" max="6" style="30" width="14.453125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="30" width="23.08984375" collapsed="true"/>
-    <col min="8" max="9" style="30" width="14.453125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="30" width="29.7265625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="30" width="17.7265625" collapsed="true"/>
-    <col min="12" max="16384" style="30" width="14.453125" collapsed="true"/>
+    <col min="1" max="1" style="29" width="14.453125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="29" width="22.54296875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="29" width="11.26953125" collapsed="true"/>
+    <col min="4" max="6" style="29" width="14.453125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="29" width="23.08984375" collapsed="true"/>
+    <col min="8" max="9" style="29" width="14.453125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="29" width="29.7265625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="29" width="17.7265625" collapsed="true"/>
+    <col min="12" max="16384" style="29" width="14.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="23" t="s">
         <v>29</v>
       </c>
       <c r="K1" s="4" t="s">
@@ -5583,364 +5593,364 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="27" t="s">
+        <v>398</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>399</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>400</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>401</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>402</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>403</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>404</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>405</v>
+      </c>
+      <c r="H6" s="31" t="s">
         <v>406</v>
       </c>
-      <c r="H2" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="27" t="s">
+      <c r="I6" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>407</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>408</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>409</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>410</v>
+      </c>
+      <c r="I8" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J8" s="26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>411</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>412</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>413</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>414</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="27" t="s">
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>415</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>416</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="L2" s="27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>407</v>
-      </c>
-      <c r="H3" s="34" t="s">
-        <v>408</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="J3" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="L3" s="27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>409</v>
-      </c>
-      <c r="H4" s="34" t="s">
-        <v>410</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="J4" s="27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>411</v>
-      </c>
-      <c r="H5" s="34" t="s">
-        <v>412</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>413</v>
-      </c>
-      <c r="H6" s="34" t="s">
-        <v>414</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="J6" s="27" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="G7" s="28" t="s">
-        <v>415</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>416</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="J7" s="27" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="G8" s="28" t="s">
-        <v>417</v>
-      </c>
-      <c r="H8" s="34" t="s">
-        <v>418</v>
-      </c>
-      <c r="I8" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="J8" s="27" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="G9" s="28" t="s">
-        <v>419</v>
-      </c>
-      <c r="H9" s="34" t="s">
-        <v>420</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="J9" s="27" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>421</v>
-      </c>
-      <c r="H10" s="34" t="s">
-        <v>422</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="J10" s="27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>423</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>424</v>
-      </c>
-      <c r="I11" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="J11" s="27" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27" t="s">
+      <c r="E12" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="F12" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="G12" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="H12" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="I12" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="J12" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="27" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I13" s="27" t="s">
+      <c r="I13" s="26" t="s">
         <v>57</v>
       </c>
     </row>
@@ -5962,31 +5972,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" style="30" width="14.453125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="30" width="17.453125" collapsed="true"/>
-    <col min="7" max="16384" style="30" width="14.453125" collapsed="true"/>
+    <col min="1" max="5" style="29" width="14.453125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="29" width="17.453125" collapsed="true"/>
+    <col min="7" max="16384" style="29" width="14.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
         <v>8</v>
       </c>
       <c r="H1" s="6" t="s">
@@ -5994,235 +6004,235 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="29" t="s">
+      <c r="D2" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="26" t="s">
         <v>172</v>
       </c>
       <c r="H2" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="27" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="13" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="D4" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="29" t="s">
+      <c r="D4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="27" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="D5" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="29" t="s">
+      <c r="D5" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="27" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="D6" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="29" t="s">
+      <c r="D6" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="27" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="D7" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="29" t="s">
+      <c r="D7" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="27" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="D8" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="29" t="s">
+      <c r="D8" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="27" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="D9" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="29" t="s">
+      <c r="D9" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="27" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="29" t="s">
+      <c r="D10" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="27" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="D11" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="29" t="s">
+      <c r="D11" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="27" t="s">
         <v>186</v>
       </c>
     </row>
@@ -6235,8 +6245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51735CCE-AD12-41B8-BE1D-C09549EADDDD}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6246,8 +6256,7 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="9.1796875" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="14.08984375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" width="15.1796875" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="27.54296875" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="8.36328125" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
@@ -6274,34 +6283,34 @@
         <v>8</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G1" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>321</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>322</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>323</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>324</v>
       </c>
       <c r="K1" s="18" t="s">
         <v>31</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -6312,7 +6321,7 @@
         <v>261</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>41</v>
@@ -6321,19 +6330,19 @@
         <v>43</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>386</v>
-      </c>
-      <c r="H2" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>384</v>
+      </c>
+      <c r="H2" s="31" t="s">
         <v>385</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -6344,7 +6353,7 @@
         <v>261</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>41</v>
@@ -6353,19 +6362,19 @@
         <v>43</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>312</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>387</v>
-      </c>
-      <c r="H3" s="22" t="s">
-        <v>388</v>
+        <v>309</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>384</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>385</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -6376,7 +6385,7 @@
         <v>261</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>41</v>
@@ -6385,19 +6394,19 @@
         <v>43</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="G4" s="22">
-        <v>44353</v>
-      </c>
-      <c r="H4" s="22">
-        <v>44359</v>
+        <v>310</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>386</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>387</v>
       </c>
       <c r="I4" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>327</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -6408,7 +6417,7 @@
         <v>261</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>41</v>
@@ -6417,19 +6426,19 @@
         <v>43</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="G5" s="22">
-        <v>44195</v>
-      </c>
-      <c r="H5" s="22">
-        <v>44199</v>
+        <v>311</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>388</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>389</v>
       </c>
       <c r="I5" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>328</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -6440,7 +6449,7 @@
         <v>261</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>41</v>
@@ -6449,19 +6458,19 @@
         <v>43</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="G6" s="22">
-        <v>44496</v>
-      </c>
-      <c r="H6" s="22">
-        <v>44501</v>
+        <v>312</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>390</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>391</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -6472,7 +6481,7 @@
         <v>261</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>41</v>
@@ -6481,19 +6490,19 @@
         <v>43</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="G7" s="22">
-        <v>44086</v>
-      </c>
-      <c r="H7" s="22">
-        <v>44088</v>
+        <v>313</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>392</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>388</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -6504,7 +6513,7 @@
         <v>261</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>41</v>
@@ -6513,19 +6522,19 @@
         <v>43</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="G8" s="22">
-        <v>44513</v>
-      </c>
-      <c r="H8" s="22">
-        <v>44515</v>
+        <v>314</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>393</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>388</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -6536,7 +6545,7 @@
         <v>261</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>41</v>
@@ -6545,19 +6554,19 @@
         <v>43</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="G9" s="22">
-        <v>44176</v>
-      </c>
-      <c r="H9" s="22">
-        <v>44180</v>
+        <v>315</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>394</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>395</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -6568,7 +6577,7 @@
         <v>261</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>41</v>
@@ -6577,19 +6586,19 @@
         <v>43</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="G10" s="22">
-        <v>44321</v>
-      </c>
-      <c r="H10" s="22">
-        <v>44335</v>
+        <v>316</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>393</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>388</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -6600,7 +6609,7 @@
         <v>261</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>41</v>
@@ -6609,19 +6618,19 @@
         <v>43</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="G11" s="22">
-        <v>44083</v>
-      </c>
-      <c r="H11" s="22">
-        <v>44114</v>
+        <v>317</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>396</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>397</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BaseClass is added, Pass and Failure mechanism introduced
</commit_message>
<xml_diff>
--- a/test-resources/HRM_TestData.xlsx
+++ b/test-resources/HRM_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schakil\git\OrangeHRMAutomation\test-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01457401-2AFA-4572-A612-3FC49B8408E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF1E6E8-F25F-4BE4-B693-21D6B86A9D6F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="491">
   <si>
     <t>S. No</t>
   </si>
@@ -2008,7 +2008,7 @@
   <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2134,12 +2134,18 @@
         <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="2"/>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">

</xml_diff>

<commit_message>
Added Login Data and made changes in Excel file.
</commit_message>
<xml_diff>
--- a/test-resources/HRM_TestData.xlsx
+++ b/test-resources/HRM_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schakil\git\OrangeHRMAutomation\test-resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aneesh\git\OrangeHRMAutomation\test-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D801DA20-0070-400B-82A8-76E462AC7B8A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0C3B68-ECA2-4F08-A0EF-354D09134ACE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="507">
   <si>
     <t>S. No</t>
   </si>
@@ -1543,17 +1543,23 @@
     <t>Orange HRM Application Login and Logout</t>
   </si>
   <si>
-    <t>alice</t>
-  </si>
-  <si>
-    <t>Test123</t>
+    <t>New User Name</t>
+  </si>
+  <si>
+    <t>New Password</t>
+  </si>
+  <si>
+    <t>liza123</t>
+  </si>
+  <si>
+    <t>nHppVDh3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1577,6 +1583,10 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -1732,10 +1742,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1827,11 +1838,18 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2129,7 +2147,7 @@
         <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>133</v>
+        <v>14</v>
       </c>
       <c r="I3" s="3"/>
     </row>
@@ -2154,7 +2172,7 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" t="s">
-        <v>133</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2573,17 +2591,17 @@
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:9" s="23" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="45"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="47"/>
     </row>
     <row r="25" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -2806,17 +2824,17 @@
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:9" s="23" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="45"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="45"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="47"/>
     </row>
     <row r="36" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
@@ -3049,17 +3067,17 @@
       <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:9" s="23" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="B46" s="44"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="45"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="47"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="47"/>
     </row>
     <row r="47" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
@@ -3278,17 +3296,17 @@
       <c r="G56" s="2"/>
     </row>
     <row r="57" spans="1:9" s="23" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="43" t="s">
+      <c r="A57" s="45" t="s">
         <v>182</v>
       </c>
-      <c r="B57" s="44"/>
-      <c r="C57" s="44"/>
-      <c r="D57" s="44"/>
-      <c r="E57" s="44"/>
-      <c r="F57" s="44"/>
-      <c r="G57" s="45"/>
-      <c r="H57" s="44"/>
-      <c r="I57" s="45"/>
+      <c r="B57" s="46"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="47"/>
+      <c r="H57" s="46"/>
+      <c r="I57" s="47"/>
     </row>
     <row r="58" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
@@ -3507,17 +3525,17 @@
       <c r="G67" s="2"/>
     </row>
     <row r="68" spans="1:9" s="23" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="43" t="s">
+      <c r="A68" s="45" t="s">
         <v>207</v>
       </c>
-      <c r="B68" s="44"/>
-      <c r="C68" s="44"/>
-      <c r="D68" s="44"/>
-      <c r="E68" s="44"/>
-      <c r="F68" s="44"/>
-      <c r="G68" s="45"/>
-      <c r="H68" s="44"/>
-      <c r="I68" s="45"/>
+      <c r="B68" s="46"/>
+      <c r="C68" s="46"/>
+      <c r="D68" s="46"/>
+      <c r="E68" s="46"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="47"/>
+      <c r="H68" s="46"/>
+      <c r="I68" s="47"/>
     </row>
     <row r="69" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
@@ -3736,17 +3754,17 @@
       <c r="G78" s="2"/>
     </row>
     <row r="79" spans="1:9" s="23" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="43" t="s">
+      <c r="A79" s="45" t="s">
         <v>231</v>
       </c>
-      <c r="B79" s="44"/>
-      <c r="C79" s="44"/>
-      <c r="D79" s="44"/>
-      <c r="E79" s="44"/>
-      <c r="F79" s="44"/>
-      <c r="G79" s="45"/>
-      <c r="H79" s="44"/>
-      <c r="I79" s="45"/>
+      <c r="B79" s="46"/>
+      <c r="C79" s="46"/>
+      <c r="D79" s="46"/>
+      <c r="E79" s="46"/>
+      <c r="F79" s="46"/>
+      <c r="G79" s="47"/>
+      <c r="H79" s="46"/>
+      <c r="I79" s="47"/>
     </row>
     <row r="80" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
@@ -3959,17 +3977,17 @@
       <c r="G89" s="2"/>
     </row>
     <row r="90" spans="1:9" s="23" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="43" t="s">
+      <c r="A90" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="B90" s="44"/>
-      <c r="C90" s="44"/>
-      <c r="D90" s="44"/>
-      <c r="E90" s="44"/>
-      <c r="F90" s="44"/>
-      <c r="G90" s="45"/>
-      <c r="H90" s="44"/>
-      <c r="I90" s="45"/>
+      <c r="B90" s="46"/>
+      <c r="C90" s="46"/>
+      <c r="D90" s="46"/>
+      <c r="E90" s="46"/>
+      <c r="F90" s="46"/>
+      <c r="G90" s="47"/>
+      <c r="H90" s="46"/>
+      <c r="I90" s="47"/>
     </row>
     <row r="91" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
@@ -5646,10 +5664,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D79F735-DD97-416B-B04A-A8B3BF03F3F1}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5657,9 +5675,11 @@
     <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="23.54296875" customWidth="1" collapsed="1"/>
     <col min="3" max="5" width="10.81640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -5669,14 +5689,20 @@
       <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="43" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="8" t="s">
+        <v>503</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
@@ -5687,13 +5713,19 @@
         <v>492</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>503</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>34</v>
       </c>
@@ -5706,11 +5738,13 @@
       <c r="D3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="44" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="4"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
@@ -5723,11 +5757,13 @@
       <c r="D4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="44" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="4"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
@@ -5740,11 +5776,13 @@
       <c r="D5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="44" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="4"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>41</v>
       </c>
@@ -5757,11 +5795,13 @@
       <c r="D6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="44" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="4"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>43</v>
       </c>
@@ -5774,11 +5814,13 @@
       <c r="D7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="44" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="4"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
@@ -5791,11 +5833,13 @@
       <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="44" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="4"/>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>48</v>
       </c>
@@ -5808,11 +5852,13 @@
       <c r="D9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="44" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="4"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>51</v>
       </c>
@@ -5825,11 +5871,13 @@
       <c r="D10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="44" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="4"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>54</v>
       </c>
@@ -5842,13 +5890,17 @@
       <c r="D11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="44" t="s">
         <v>31</v>
       </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="10"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="Admin@123" xr:uid="{FDDD0EE2-7999-4245-8E7D-D928FF2B0B5B}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{7BD59133-5984-4A1A-A9F3-B7E14A6C8529}"/>
+    <hyperlink ref="E3:E11" r:id="rId2" display="Admin@123" xr:uid="{E7F63DB0-782E-41D5-89BD-08F576A6326F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Made changes in AddLoginData
</commit_message>
<xml_diff>
--- a/test-resources/HRM_TestData.xlsx
+++ b/test-resources/HRM_TestData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aneesh\git\OrangeHRMAutomation\test-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0C3B68-ECA2-4F08-A0EF-354D09134ACE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86CE5A5-E60B-4516-9562-56DD2C194F4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="535">
   <si>
     <t>S. No</t>
   </si>
@@ -1543,22 +1543,107 @@
     <t>Orange HRM Application Login and Logout</t>
   </si>
   <si>
-    <t>New User Name</t>
-  </si>
-  <si>
-    <t>New Password</t>
+    <t>PRUSwNjw</t>
+  </si>
+  <si>
+    <t>emily.harris</t>
+  </si>
+  <si>
+    <t>tybWaSiM</t>
+  </si>
+  <si>
+    <t>george.tofari</t>
+  </si>
+  <si>
+    <t>GEAIYDdC</t>
+  </si>
+  <si>
+    <t>jendayi.jumoke</t>
+  </si>
+  <si>
+    <t>42Gmt7CO</t>
+  </si>
+  <si>
+    <t>gkFGZuVn</t>
+  </si>
+  <si>
+    <t>chenzira.chuki</t>
+  </si>
+  <si>
+    <t>6TKk6ozB</t>
+  </si>
+  <si>
+    <t>jacqueline.white</t>
+  </si>
+  <si>
+    <t>zfBsbNyE</t>
   </si>
   <si>
     <t>liza123</t>
   </si>
   <si>
-    <t>nHppVDh3</t>
+    <t>Z2SeK3UX</t>
+  </si>
+  <si>
+    <t>linda</t>
+  </si>
+  <si>
+    <t>RJjG4VWQ</t>
+  </si>
+  <si>
+    <t>khloe.jayden</t>
+  </si>
+  <si>
+    <t>Zu7oqFiq</t>
+  </si>
+  <si>
+    <t>Kx9C1MjG</t>
+  </si>
+  <si>
+    <t>johns</t>
+  </si>
+  <si>
+    <t>97WTid1I</t>
+  </si>
+  <si>
+    <t>kiyara.hu</t>
+  </si>
+  <si>
+    <t>59XQ7iOI</t>
+  </si>
+  <si>
+    <t>fisher</t>
+  </si>
+  <si>
+    <t>ZWWFSXab</t>
+  </si>
+  <si>
+    <t>4xdFk8Ti</t>
+  </si>
+  <si>
+    <t>uDYj1ZpW</t>
+  </si>
+  <si>
+    <t>jadine.jackie</t>
+  </si>
+  <si>
+    <t>4pO4pF9V</t>
+  </si>
+  <si>
+    <t>loiuse.anderson</t>
+  </si>
+  <si>
+    <t>BtfMqDJm</t>
+  </si>
+  <si>
+    <t>fiona.grace</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1590,7 +1675,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1661,6 +1746,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -1746,7 +1837,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1847,6 +1938,15 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2074,15 +2174,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.54296875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="35.90625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.81640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="65.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.26953125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.54296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="35.90625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.26953125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.90625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="65.6328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="19" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4222,7 +4322,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
@@ -4230,21 +4330,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.08984375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.81640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.08984375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.54296875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.08984375" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="15.08984375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="27.54296875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8.453125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.26953125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.81640625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.08984375" customWidth="1" collapsed="1"/>
-    <col min="16" max="26" width="8.7265625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.08984375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.08984375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="10.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.08984375" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="15.08984375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="27.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="8.453125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.26953125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="9.81640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="16" max="26" customWidth="true" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -5667,16 +5767,16 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.54296875" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="10.81640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.54296875" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.90625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5695,12 +5795,8 @@
       <c r="E1" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>503</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>504</v>
-      </c>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -5713,17 +5809,13 @@
         <v>492</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>30</v>
+        <v>519</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>506</v>
-      </c>
+        <v>518</v>
+      </c>
+      <c r="F2" s="49"/>
+      <c r="G2" s="50"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -5736,10 +5828,10 @@
         <v>493</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>30</v>
+        <v>515</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>31</v>
+        <v>520</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="10"/>
@@ -5755,10 +5847,10 @@
         <v>494</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>30</v>
+        <v>522</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>31</v>
+        <v>521</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="10"/>
@@ -5774,10 +5866,10 @@
         <v>495</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>30</v>
+        <v>524</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>31</v>
+        <v>523</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="10"/>
@@ -5793,10 +5885,10 @@
         <v>496</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>30</v>
+        <v>526</v>
       </c>
       <c r="E6" s="44" t="s">
-        <v>31</v>
+        <v>525</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="10"/>
@@ -5812,10 +5904,10 @@
         <v>497</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>30</v>
+        <v>508</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>31</v>
+        <v>527</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="10"/>
@@ -5831,10 +5923,10 @@
         <v>498</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>30</v>
+        <v>506</v>
       </c>
       <c r="E8" s="44" t="s">
-        <v>31</v>
+        <v>528</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="10"/>
@@ -5850,10 +5942,10 @@
         <v>499</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>30</v>
+        <v>530</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>31</v>
+        <v>529</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="10"/>
@@ -5869,10 +5961,10 @@
         <v>500</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>30</v>
+        <v>532</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>31</v>
+        <v>531</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="10"/>
@@ -5888,10 +5980,10 @@
         <v>501</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>30</v>
+        <v>534</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>31</v>
+        <v>533</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="10"/>
@@ -5908,7 +6000,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Q1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
@@ -5916,21 +6008,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.54296875" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="10.81640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.54296875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.26953125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.453125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="28.54296875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="27.453125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.81640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.453125" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="8.7265625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="19.54296875" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="26" width="8.7265625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.54296875" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="9.54296875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.26953125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="28.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="27.453125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.453125" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="8.7265625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="19.54296875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.08984375" collapsed="true"/>
+    <col min="18" max="26" customWidth="true" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -7484,17 +7576,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.26953125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.81640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7265625" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.54296875" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.453125" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.453125" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.7265625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.1796875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="26" width="8.7265625" style="4" customWidth="1" collapsed="1"/>
-    <col min="27" max="16384" width="14.453125" style="4" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="19.26953125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="10.81640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="9.7265625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="10.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="25.453125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="19.453125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="4" width="16.7265625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="4" width="18.1796875" collapsed="true"/>
+    <col min="10" max="26" customWidth="true" style="4" width="8.7265625" collapsed="true"/>
+    <col min="27" max="16384" style="4" width="14.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -8747,19 +8839,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.54296875" style="29" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.81640625" style="29" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.08984375" style="29" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.54296875" style="29" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.08984375" style="29" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.26953125" style="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.453125" style="29" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.54296875" style="29" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.453125" style="29" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.08984375" style="29" customWidth="1" collapsed="1"/>
-    <col min="12" max="26" width="8.7265625" style="29" customWidth="1" collapsed="1"/>
-    <col min="27" max="16384" width="14.453125" style="29" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="29" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="29" width="22.54296875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="29" width="10.81640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="29" width="9.08984375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="29" width="10.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="29" width="13.08984375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="29" width="21.26953125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="29" width="25.453125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="29" width="14.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="29" width="21.453125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="29" width="12.08984375" collapsed="true"/>
+    <col min="12" max="26" customWidth="true" style="29" width="8.7265625" collapsed="true"/>
+    <col min="27" max="16384" style="29" width="14.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -10129,17 +10221,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.36328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.1796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.26953125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.36328125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="22.54296875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10576,15 +10668,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.81640625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.90625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.90625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.54296875" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.26953125" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="14.453125" style="29" collapsed="1"/>
-    <col min="9" max="9" width="15.7265625" style="29" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="14.453125" style="29" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="29" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="29" width="21.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="29" width="10.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="29" width="8.90625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="29" width="10.54296875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="29" width="19.26953125" collapsed="true"/>
+    <col min="7" max="8" style="29" width="14.453125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="29" width="15.7265625" collapsed="true"/>
+    <col min="10" max="16384" style="29" width="14.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10925,13 +11017,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.453125" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="14.453125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.36328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.90625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.453125" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="14.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11419,17 +11511,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.08984375" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="14.453125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.7265625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.7265625" customWidth="1" collapsed="1"/>
-    <col min="12" max="14" width="14.453125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.54296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.1796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="23.08984375" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="29.7265625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="17.7265625" collapsed="true"/>
+    <col min="12" max="14" customWidth="true" width="14.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made changes in testcases
</commit_message>
<xml_diff>
--- a/test-resources/HRM_TestData.xlsx
+++ b/test-resources/HRM_TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aneesh\git\OrangeHRMAutomation\test-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F34AECB-DD78-4C37-9EDA-2A734E4A9213}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC4B725-21EA-441C-9B41-FA0DAB592FA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="755" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="755" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="507">
   <si>
     <t>S. No</t>
   </si>
@@ -1541,12 +1541,25 @@
   </si>
   <si>
     <t>TC_02_EditLocation</t>
+  </si>
+  <si>
+    <t>AustraliaLumivX</t>
+  </si>
+  <si>
+    <t>Actual value is not matched with Expected value :OrangeHRM</t>
+  </si>
+  <si>
+    <t>John Adam fnsf</t>
+  </si>
+  <si>
+    <t>1002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1841,9 +1854,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1857,6 +1867,9 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2084,15 +2097,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.54296875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="35.90625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.81640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="65.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.26953125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.54296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="35.90625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.26953125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.90625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="65.6328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="19" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2442,7 +2455,7 @@
         <v>133</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>134</v>
+        <v>504</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2651,17 +2664,17 @@
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:9" s="23" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="46"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="51"/>
     </row>
     <row r="25" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -2884,17 +2897,17 @@
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:9" s="23" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="46"/>
-      <c r="H35" s="45"/>
-      <c r="I35" s="46"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="51"/>
     </row>
     <row r="36" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
@@ -3127,17 +3140,17 @@
       <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:9" s="23" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="44" t="s">
+      <c r="A46" s="49" t="s">
         <v>160</v>
       </c>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="46"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="46"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="50"/>
+      <c r="I46" s="51"/>
     </row>
     <row r="47" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
@@ -3356,17 +3369,17 @@
       <c r="G56" s="2"/>
     </row>
     <row r="57" spans="1:9" s="23" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="44" t="s">
+      <c r="A57" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="B57" s="45"/>
-      <c r="C57" s="45"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="45"/>
-      <c r="F57" s="45"/>
-      <c r="G57" s="46"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="46"/>
+      <c r="B57" s="50"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
+      <c r="E57" s="50"/>
+      <c r="F57" s="50"/>
+      <c r="G57" s="51"/>
+      <c r="H57" s="50"/>
+      <c r="I57" s="51"/>
     </row>
     <row r="58" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
@@ -3585,17 +3598,17 @@
       <c r="G67" s="2"/>
     </row>
     <row r="68" spans="1:9" s="23" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="44" t="s">
+      <c r="A68" s="49" t="s">
         <v>207</v>
       </c>
-      <c r="B68" s="45"/>
-      <c r="C68" s="45"/>
-      <c r="D68" s="45"/>
-      <c r="E68" s="45"/>
-      <c r="F68" s="45"/>
-      <c r="G68" s="46"/>
-      <c r="H68" s="45"/>
-      <c r="I68" s="46"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="50"/>
+      <c r="E68" s="50"/>
+      <c r="F68" s="50"/>
+      <c r="G68" s="51"/>
+      <c r="H68" s="50"/>
+      <c r="I68" s="51"/>
     </row>
     <row r="69" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
@@ -3814,17 +3827,17 @@
       <c r="G78" s="2"/>
     </row>
     <row r="79" spans="1:9" s="23" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="44" t="s">
+      <c r="A79" s="49" t="s">
         <v>231</v>
       </c>
-      <c r="B79" s="45"/>
-      <c r="C79" s="45"/>
-      <c r="D79" s="45"/>
-      <c r="E79" s="45"/>
-      <c r="F79" s="45"/>
-      <c r="G79" s="46"/>
-      <c r="H79" s="45"/>
-      <c r="I79" s="46"/>
+      <c r="B79" s="50"/>
+      <c r="C79" s="50"/>
+      <c r="D79" s="50"/>
+      <c r="E79" s="50"/>
+      <c r="F79" s="50"/>
+      <c r="G79" s="51"/>
+      <c r="H79" s="50"/>
+      <c r="I79" s="51"/>
     </row>
     <row r="80" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
@@ -4037,17 +4050,17 @@
       <c r="G89" s="2"/>
     </row>
     <row r="90" spans="1:9" s="23" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="44" t="s">
+      <c r="A90" s="49" t="s">
         <v>242</v>
       </c>
-      <c r="B90" s="45"/>
-      <c r="C90" s="45"/>
-      <c r="D90" s="45"/>
-      <c r="E90" s="45"/>
-      <c r="F90" s="45"/>
-      <c r="G90" s="46"/>
-      <c r="H90" s="45"/>
-      <c r="I90" s="46"/>
+      <c r="B90" s="50"/>
+      <c r="C90" s="50"/>
+      <c r="D90" s="50"/>
+      <c r="E90" s="50"/>
+      <c r="F90" s="50"/>
+      <c r="G90" s="51"/>
+      <c r="H90" s="50"/>
+      <c r="I90" s="51"/>
     </row>
     <row r="91" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
@@ -4282,7 +4295,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
@@ -4290,21 +4303,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.08984375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.81640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.08984375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.54296875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.08984375" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="15.08984375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="27.54296875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8.453125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.26953125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.81640625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.08984375" customWidth="1" collapsed="1"/>
-    <col min="16" max="26" width="8.7265625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.08984375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.08984375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="10.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.08984375" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="15.08984375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="27.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="8.453125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.26953125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="9.81640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="16" max="26" customWidth="true" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -5732,11 +5745,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.54296875" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="10.81640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.54296875" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.90625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5749,14 +5762,14 @@
       <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -5770,8 +5783,8 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="43"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="49"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="46"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -5916,29 +5929,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.54296875" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="10.81640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.54296875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.26953125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.453125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="28.54296875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="27.453125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.81640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.453125" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="8.7265625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="19.54296875" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="26" width="8.7265625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.54296875" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="9.54296875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.26953125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="28.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="27.453125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.453125" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="8.7265625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="19.54296875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.08984375" collapsed="true"/>
+    <col min="18" max="26" customWidth="true" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -6019,8 +6032,8 @@
       <c r="H2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>50</v>
+      <c r="I2" s="29" t="s">
+        <v>503</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>70</v>
@@ -6040,8 +6053,12 @@
       <c r="O2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
+      <c r="P2" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="3" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -7492,17 +7509,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.26953125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.81640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7265625" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.54296875" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.453125" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.453125" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.7265625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.1796875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="26" width="8.7265625" style="4" customWidth="1" collapsed="1"/>
-    <col min="27" max="16384" width="14.453125" style="4" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="19.26953125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="10.81640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="9.7265625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="10.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="25.453125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="19.453125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="4" width="16.7265625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="4" width="18.1796875" collapsed="true"/>
+    <col min="10" max="26" customWidth="true" style="4" width="8.7265625" collapsed="true"/>
+    <col min="27" max="16384" style="4" width="14.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -8749,25 +8766,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.54296875" style="29" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.81640625" style="29" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.08984375" style="29" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.54296875" style="29" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.08984375" style="29" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.26953125" style="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.453125" style="29" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.54296875" style="29" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.453125" style="29" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.08984375" style="29" customWidth="1" collapsed="1"/>
-    <col min="12" max="26" width="8.7265625" style="29" customWidth="1" collapsed="1"/>
-    <col min="27" max="16384" width="14.453125" style="29" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="29" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="29" width="22.54296875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="29" width="10.81640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="29" width="9.08984375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="29" width="10.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="29" width="13.08984375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="29" width="21.26953125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="29" width="25.453125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="29" width="14.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="29" width="21.453125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="29" width="12.08984375" collapsed="true"/>
+    <col min="12" max="26" customWidth="true" style="29" width="8.7265625" collapsed="true"/>
+    <col min="27" max="16384" style="29" width="14.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -8821,11 +8838,12 @@
       <c r="E2" s="30" t="s">
         <v>31</v>
       </c>
+      <c r="F2"/>
       <c r="G2" s="29" t="s">
         <v>150</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>69</v>
+        <v>503</v>
       </c>
       <c r="I2" s="29" t="s">
         <v>152</v>
@@ -8833,8 +8851,8 @@
       <c r="J2" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="K2" s="29">
-        <v>4</v>
+      <c r="K2" s="28" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -8865,8 +8883,8 @@
       <c r="J3" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="K3" s="29">
-        <v>5</v>
+      <c r="K3" s="28" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -8898,8 +8916,8 @@
       <c r="J4" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="K4" s="29">
-        <v>2</v>
+      <c r="K4" s="28" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -8930,8 +8948,8 @@
       <c r="J5" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="K5" s="29">
-        <v>2</v>
+      <c r="K5" s="28" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -8962,8 +8980,8 @@
       <c r="J6" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="K6" s="29">
-        <v>1</v>
+      <c r="K6" s="28" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -8994,8 +9012,8 @@
       <c r="J7" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="K7" s="29">
-        <v>3</v>
+      <c r="K7" s="28" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -9026,8 +9044,8 @@
       <c r="J8" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="K8" s="29">
-        <v>2</v>
+      <c r="K8" s="28" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -9058,8 +9076,8 @@
       <c r="J9" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="K9" s="29">
-        <v>5</v>
+      <c r="K9" s="28" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -9090,8 +9108,8 @@
       <c r="J10" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="K10" s="29">
-        <v>3</v>
+      <c r="K10" s="28" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -9122,8 +9140,8 @@
       <c r="J11" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="K11" s="29">
-        <v>2</v>
+      <c r="K11" s="28" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10137,17 +10155,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.36328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.1796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.26953125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.36328125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="22.54296875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10184,10 +10202,10 @@
       <c r="K1" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="47" t="s">
         <v>319</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="M1" s="47" t="s">
         <v>479</v>
       </c>
     </row>
@@ -10590,15 +10608,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.81640625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.90625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.90625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.54296875" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.26953125" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="14.453125" style="29" collapsed="1"/>
-    <col min="9" max="9" width="15.7265625" style="29" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="14.453125" style="29" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="29" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="29" width="21.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="29" width="10.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="29" width="8.90625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="29" width="10.54296875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="29" width="19.26953125" collapsed="true"/>
+    <col min="7" max="8" style="29" width="14.453125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="29" width="15.7265625" collapsed="true"/>
+    <col min="10" max="16384" style="29" width="14.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10933,19 +10951,19 @@
   </sheetPr>
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.453125" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="14.453125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.36328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.90625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.453125" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="14.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11433,17 +11451,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.08984375" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="14.453125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.7265625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.7265625" customWidth="1" collapsed="1"/>
-    <col min="12" max="14" width="14.453125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.54296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.1796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="23.08984375" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="29.7265625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="17.7265625" collapsed="true"/>
+    <col min="12" max="14" customWidth="true" width="14.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made changes in test cases and corresponding pages
</commit_message>
<xml_diff>
--- a/test-resources/HRM_TestData.xlsx
+++ b/test-resources/HRM_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aneesh\git\OrangeHRMAutomation\test-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC4B725-21EA-441C-9B41-FA0DAB592FA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B6A126-8473-48D8-9896-598C3E1D29A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="755" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="755" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="509">
   <si>
     <t>S. No</t>
   </si>
@@ -1549,10 +1549,16 @@
     <t>Actual value is not matched with Expected value :OrangeHRM</t>
   </si>
   <si>
-    <t>John Adam fnsf</t>
-  </si>
-  <si>
     <t>1002</t>
+  </si>
+  <si>
+    <t>John Adam Nilf</t>
+  </si>
+  <si>
+    <t>CanadaUNGhNB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air Ticket </t>
   </si>
 </sst>
 </file>
@@ -2699,11 +2705,9 @@
         <v>408</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>134</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
@@ -4084,9 +4088,7 @@
       <c r="H91" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I91" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="I91" s="3"/>
     </row>
     <row r="92" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
@@ -4297,8 +4299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4393,7 +4395,7 @@
         <v>269</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>390</v>
+        <v>508</v>
       </c>
       <c r="J2" s="29" t="s">
         <v>391</v>
@@ -5931,7 +5933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -6033,7 +6035,7 @@
         <v>68</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>70</v>
@@ -6054,10 +6056,10 @@
         <v>75</v>
       </c>
       <c r="P2" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>505</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made changes in test case 02 and relative pages
</commit_message>
<xml_diff>
--- a/test-resources/HRM_TestData.xlsx
+++ b/test-resources/HRM_TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="514">
   <si>
     <t>S. No</t>
   </si>
@@ -1559,6 +1559,21 @@
   </si>
   <si>
     <t xml:space="preserve">Air Ticket </t>
+  </si>
+  <si>
+    <t>South AfricaDjWOXw</t>
+  </si>
+  <si>
+    <t>John geYJ Williams</t>
+  </si>
+  <si>
+    <t>6906137415</t>
+  </si>
+  <si>
+    <t>John Adam gXUc</t>
+  </si>
+  <si>
+    <t>FrancesbhHja</t>
   </si>
 </sst>
 </file>
@@ -2705,9 +2720,11 @@
         <v>408</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" s="3"/>
+        <v>133</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
@@ -2934,11 +2951,9 @@
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>134</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
@@ -6035,7 +6050,7 @@
         <v>68</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>70</v>
@@ -6056,7 +6071,7 @@
         <v>75</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>505</v>
@@ -6480,7 +6495,7 @@
         <v>129</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>130</v>
+        <v>509</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>79</v>
@@ -7569,12 +7584,18 @@
       <c r="E2" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="30"/>
+      <c r="F2" s="30" t="s">
+        <v>130</v>
+      </c>
       <c r="G2" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
+        <v>509</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>511</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>510</v>
+      </c>
       <c r="M2" s="24"/>
     </row>
     <row r="3" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Latest Framework changes for chrome headless and some fixes.
</commit_message>
<xml_diff>
--- a/test-resources/HRM_TestData.xlsx
+++ b/test-resources/HRM_TestData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schakil\git\OrangeHRMAutomation\test-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF07BC5-5FAB-4B42-BA9D-C4278ECA0A08}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D175612F-4C70-42AA-8897-9F96FC36197A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="514">
   <si>
     <t>S. No</t>
   </si>
@@ -1564,26 +1564,22 @@
     <t>0073</t>
   </si>
   <si>
-    <t>John Adam FIQl</t>
-  </si>
-  <si>
-    <t>0062</t>
-  </si>
-  <si>
-    <t>GermanyWMEvnx</t>
-  </si>
-  <si>
-    <t>John Adam oReG</t>
-  </si>
-  <si>
-    <t>FrancesbhHja</t>
+    <t>OrangeHRM is not matched with OrangeHRM</t>
+  </si>
+  <si>
+    <t>0044</t>
+  </si>
+  <si>
+    <t>John Adam smZh</t>
+  </si>
+  <si>
+    <t>ChromeHeadless</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2115,21 +2111,21 @@
   </sheetPr>
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="I95" sqref="I95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.26953125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.54296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="35.90625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.26953125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.90625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="65.6328125" collapsed="true"/>
+    <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="35.90625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.81640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="65.6328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="19" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2193,8 +2189,8 @@
       <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
-        <v>407</v>
+      <c r="G3" s="2" t="s">
+        <v>488</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>132</v>
@@ -2223,7 +2219,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>407</v>
+        <v>488</v>
       </c>
       <c r="H4" t="s">
         <v>132</v>
@@ -2475,16 +2471,19 @@
         <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>12</v>
+        <v>513</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G14" t="s">
+        <v>407</v>
+      </c>
       <c r="H14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2957,7 +2956,9 @@
       <c r="F36" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="3"/>
+      <c r="G36" s="1" t="s">
+        <v>407</v>
+      </c>
       <c r="H36" s="3" t="s">
         <v>14</v>
       </c>
@@ -3193,17 +3194,19 @@
         <v>163</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>12</v>
+        <v>513</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G47" s="2"/>
+      <c r="G47" s="2" t="s">
+        <v>407</v>
+      </c>
       <c r="H47" s="3" t="s">
-        <v>132</v>
+        <v>14</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>133</v>
+        <v>510</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4108,6 +4111,7 @@
       <c r="F91" t="s">
         <v>13</v>
       </c>
+      <c r="G91" s="2"/>
       <c r="H91" s="3" t="s">
         <v>14</v>
       </c>
@@ -4320,7 +4324,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:O1000"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
@@ -4328,21 +4332,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.08984375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.81640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="9.08984375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.08984375" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="15.08984375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="27.54296875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="8.453125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="13.26953125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="9.81640625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="13.08984375" collapsed="true"/>
-    <col min="16" max="26" customWidth="true" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.08984375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.81640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.08984375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.54296875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.08984375" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="15.08984375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="27.54296875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="8.453125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.26953125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.81640625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.08984375" customWidth="1" collapsed="1"/>
+    <col min="16" max="26" width="8.7265625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -5770,11 +5774,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.54296875" collapsed="true"/>
-    <col min="3" max="5" customWidth="true" width="10.81640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.90625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="10.81640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5954,29 +5958,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q1000"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.54296875" collapsed="true"/>
-    <col min="3" max="5" customWidth="true" width="10.81640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="9.54296875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.26953125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="28.54296875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="27.453125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="10.81640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.453125" collapsed="true"/>
-    <col min="13" max="14" customWidth="true" width="8.7265625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="19.54296875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="11.08984375" collapsed="true"/>
-    <col min="18" max="26" customWidth="true" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="10.81640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.54296875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.26953125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.453125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="28.54296875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.453125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.81640625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.453125" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="8.7265625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="19.54296875" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="26" width="8.7265625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -6058,7 +6062,7 @@
         <v>67</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>514</v>
+        <v>52</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>69</v>
@@ -6079,7 +6083,7 @@
         <v>74</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>511</v>
@@ -7534,17 +7538,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="4.7265625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="19.26953125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="10.81640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="9.7265625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="4" width="10.54296875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="4" width="25.453125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="4" width="19.453125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="4" width="16.7265625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="4" width="18.1796875" collapsed="true"/>
-    <col min="10" max="26" customWidth="true" style="4" width="8.7265625" collapsed="true"/>
-    <col min="27" max="16384" style="4" width="14.453125" collapsed="true"/>
+    <col min="1" max="1" width="4.7265625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.26953125" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.81640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.7265625" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.54296875" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.453125" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.453125" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.7265625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.1796875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="26" width="8.7265625" style="4" customWidth="1" collapsed="1"/>
+    <col min="27" max="16384" width="14.453125" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -8803,19 +8807,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="29" width="4.7265625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="29" width="22.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="29" width="10.81640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="29" width="9.08984375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="29" width="10.54296875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="29" width="13.08984375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="29" width="21.26953125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="29" width="25.453125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="29" width="14.54296875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="29" width="21.453125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="29" width="12.08984375" collapsed="true"/>
-    <col min="12" max="26" customWidth="true" style="29" width="8.7265625" collapsed="true"/>
-    <col min="27" max="16384" style="29" width="14.453125" collapsed="true"/>
+    <col min="1" max="1" width="4.7265625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.54296875" style="29" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.81640625" style="29" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.08984375" style="29" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.54296875" style="29" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.08984375" style="29" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.26953125" style="29" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="25.453125" style="29" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.54296875" style="29" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.453125" style="29" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.08984375" style="29" customWidth="1" collapsed="1"/>
+    <col min="12" max="26" width="8.7265625" style="29" customWidth="1" collapsed="1"/>
+    <col min="27" max="16384" width="14.453125" style="29" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -10186,17 +10190,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.36328125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.1796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.26953125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.81640625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.36328125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="22.54296875" collapsed="true"/>
+    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10645,15 +10649,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="29" width="4.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="29" width="21.81640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="29" width="10.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="29" width="8.90625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="29" width="10.54296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="29" width="19.26953125" collapsed="true"/>
-    <col min="7" max="8" style="29" width="14.453125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="29" width="15.7265625" collapsed="true"/>
-    <col min="10" max="16384" style="29" width="14.453125" collapsed="true"/>
+    <col min="1" max="1" width="4.7265625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.81640625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.90625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.90625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.54296875" style="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.26953125" style="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="14.453125" style="29" collapsed="1"/>
+    <col min="9" max="9" width="15.7265625" style="29" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="14.453125" style="29" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10994,13 +10998,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.36328125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.90625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.453125" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="14.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11488,17 +11492,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="4.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.54296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.1796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="23.08984375" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" width="14.453125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="29.7265625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="17.7265625" collapsed="true"/>
-    <col min="12" max="14" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.08984375" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="14.453125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.7265625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.7265625" customWidth="1" collapsed="1"/>
+    <col min="12" max="14" width="14.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>